<commit_message>
Integrated SMFS tables and looked at total catches of fishes for water year 2011 to 2023.
</commit_message>
<xml_diff>
--- a/CodingMetadata.xlsx
+++ b/CodingMetadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cnewe\OneDrive\Documents\Incubator\Code\FishForesightIncubator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C22377-24AC-40A7-A14C-B8A7C0EE5BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A054E82-BF52-440C-900C-B2F5E994667B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D153133C-3D03-4930-B163-CDA3261149E5}"/>
   </bookViews>
@@ -573,12 +573,13 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>